<commit_message>
LAPR5-146 #node #implementation Changes
</commit_message>
<xml_diff>
--- a/doc/Sprint B/evaluation/g051_evaluation.xlsx
+++ b/doc/Sprint B/evaluation/g051_evaluation.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11114"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{BA74D892-8DA9-4D4D-81AA-C788021CA394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13147331-FF4D-6441-B353-AA0F35CCC15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27340" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fatura" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="nome_empresa">Fatura!$B$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Fatura!$3:$3</definedName>
     <definedName name="RegiãoDeTítuloDaLinha1..C7">Fatura!#REF!</definedName>
     <definedName name="RegiãoDeTítuloDaLinha2..G5">Fatura!#REF!</definedName>
     <definedName name="RegiãoDeTítuloDaLinha3..G26">Fatura!#REF!</definedName>
     <definedName name="TítuloDaColuna1">FaturaSimples[[#Headers],[Número do Aluno]]</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">Fatura!$3:$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="13">
   <si>
     <t>Grupo 051</t>
   </si>
@@ -70,6 +70,9 @@
   <si>
     <t>Tiago Costa</t>
   </si>
+  <si>
+    <t>Fair</t>
+  </si>
 </sst>
 </file>
 
@@ -80,7 +83,7 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="#_)"/>
-    <numFmt numFmtId="169" formatCode="[&lt;=999999999]###\ ###\ ###;\(###\)\ ###\ ###\ ###"/>
+    <numFmt numFmtId="168" formatCode="[&lt;=999999999]###\ ###\ ###;\(###\)\ ###\ ###\ ###"/>
   </numFmts>
   <fonts count="24" x14ac:knownFonts="1">
     <font>
@@ -612,7 +615,7 @@
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0">
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0">
@@ -677,89 +680,83 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="6" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="6" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="52">
-    <cellStyle name="20% - Cor1" xfId="15" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Cor2" xfId="33" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Cor3" xfId="37" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Cor4" xfId="41" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Cor5" xfId="45" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Cor6" xfId="49" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Cor1" xfId="31" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Cor2" xfId="34" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Cor3" xfId="38" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Cor4" xfId="42" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Cor5" xfId="46" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Cor6" xfId="50" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Cor1" xfId="7" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Cor2" xfId="35" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Cor3" xfId="39" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Cor4" xfId="43" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Cor5" xfId="47" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Cor6" xfId="51" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Cabeçalho 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Cabeçalho 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Cabeçalho 3" xfId="8" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Cabeçalho 4" xfId="12" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="26" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Célula Ligada" xfId="27" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Cor1" xfId="30" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Cor2" xfId="32" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Cor3" xfId="36" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Cor4" xfId="40" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Cor5" xfId="44" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Cor6" xfId="48" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Correto" xfId="21" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="15" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="33" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="37" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="45" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="49" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="31" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="34" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="38" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="46" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="50" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="7" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="35" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="39" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="43" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="47" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="51" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="30" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="32" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="36" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="44" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="48" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="22" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="28" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Comma" xfId="19" builtinId="3" customBuiltin="1"/>
+    <cellStyle name="Comma [0]" xfId="20" builtinId="6" customBuiltin="1"/>
+    <cellStyle name="Currency" xfId="13" builtinId="4" customBuiltin="1"/>
+    <cellStyle name="Currency [0]" xfId="14" builtinId="7" customBuiltin="1"/>
     <cellStyle name="Data" xfId="18" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Entrada" xfId="24" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Hiperligação" xfId="1" builtinId="8" customBuiltin="1"/>
-    <cellStyle name="Hiperligação Visitada" xfId="5" builtinId="9" customBuiltin="1"/>
-    <cellStyle name="Incorreto" xfId="22" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Moeda" xfId="13" builtinId="4" customBuiltin="1"/>
-    <cellStyle name="Moeda [0]" xfId="14" builtinId="7" customBuiltin="1"/>
-    <cellStyle name="Neutro" xfId="23" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="10" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="21" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="8" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="12" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="24" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="23" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Nota" xfId="29" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Percentagem" xfId="4" builtinId="5" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="29" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="25" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Per cent" xfId="4" builtinId="5" customBuiltin="1"/>
     <cellStyle name="Quantidade" xfId="17" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="Saída" xfId="25" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Separador de milhares [0]" xfId="20" builtinId="6" customBuiltin="1"/>
     <cellStyle name="Telefone" xfId="16" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="Texto de Aviso" xfId="9" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto Explicativo" xfId="10" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="6" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="6" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="11" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Verificar Célula" xfId="28" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Vírgula" xfId="19" builtinId="3" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="15">
     <dxf>
       <font>
         <b val="0"/>
@@ -851,25 +848,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -964,12 +946,12 @@
   </dxfs>
   <tableStyles count="1" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Fatura" pivot="0" count="6" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="17"/>
-      <tableStyleElement type="headerRow" dxfId="16"/>
-      <tableStyleElement type="totalRow" dxfId="15"/>
-      <tableStyleElement type="lastColumn" dxfId="14"/>
-      <tableStyleElement type="firstRowStripe" dxfId="13"/>
-      <tableStyleElement type="secondRowStripe" dxfId="12"/>
+      <tableStyleElement type="wholeTable" dxfId="14"/>
+      <tableStyleElement type="headerRow" dxfId="13"/>
+      <tableStyleElement type="totalRow" dxfId="12"/>
+      <tableStyleElement type="lastColumn" dxfId="11"/>
+      <tableStyleElement type="firstRowStripe" dxfId="10"/>
+      <tableStyleElement type="secondRowStripe" dxfId="9"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1052,7 +1034,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="FaturaSimples" displayName="FaturaSimples" ref="B3:H7" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="FaturaSimples" displayName="FaturaSimples" ref="B3:H7" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="B3:H7" xr:uid="{00000000-0009-0000-0100-000004000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -1063,13 +1045,13 @@
     <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Número do Aluno" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Nome" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Autoavaliação" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="1190424" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{3CD2734D-C3BF-4780-B7D9-1B2C74D68A9E}" name="1190682" dataDxfId="4" dataCellStyle="Moeda"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="1190967" dataDxfId="3" dataCellStyle="Moeda"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="191460" dataDxfId="2" dataCellStyle="Moeda"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Número do Aluno" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Nome" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Autoavaliação" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="1190424" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{3CD2734D-C3BF-4780-B7D9-1B2C74D68A9E}" name="1190682" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="1190967" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="191460" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Fatura" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1314,31 +1296,31 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="34" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.85546875" customWidth="1"/>
-    <col min="4" max="8" width="19.7109375" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.83203125" customWidth="1"/>
+    <col min="4" max="8" width="19.6640625" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="57.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="58" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7"/>
+      <c r="C1" s="13"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="6"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="44.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="44" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B2" s="3"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
@@ -1347,112 +1329,112 @@
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
+    <row r="3" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="11">
+    <row r="4" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="10">
         <v>1190424</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="12">
-        <v>19</v>
-      </c>
-      <c r="E4" s="13"/>
-      <c r="F4" s="12">
-        <v>19</v>
-      </c>
-      <c r="G4" s="12">
-        <v>19</v>
-      </c>
-      <c r="H4" s="12">
-        <v>19</v>
+      <c r="D4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="12"/>
+      <c r="F4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="11">
+    <row r="5" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="10">
         <v>1190682</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="12">
-        <v>19</v>
-      </c>
-      <c r="E5" s="12">
-        <v>19</v>
-      </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="12">
-        <v>19</v>
-      </c>
-      <c r="H5" s="12">
-        <v>19</v>
+      <c r="D5" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="11">
+    <row r="6" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="10">
         <v>1190967</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="12">
-        <v>19</v>
-      </c>
-      <c r="E6" s="12">
-        <v>19</v>
-      </c>
-      <c r="F6" s="12">
-        <v>19</v>
-      </c>
-      <c r="G6" s="13"/>
-      <c r="H6" s="12">
-        <v>19</v>
+      <c r="D6" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="12"/>
+      <c r="H6" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="11">
+    <row r="7" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="10">
         <v>191460</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="12">
-        <v>19</v>
-      </c>
-      <c r="E7" s="12">
-        <v>19</v>
-      </c>
-      <c r="F7" s="12">
-        <v>19</v>
-      </c>
-      <c r="G7" s="12">
-        <v>19</v>
-      </c>
-      <c r="H7" s="13"/>
+      <c r="D7" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="12"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" selectLockedCells="1" sort="0"/>

</xml_diff>